<commit_message>
Subida con 1 solo archivo
</commit_message>
<xml_diff>
--- a/project excel.xlsx
+++ b/project excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lfern\Desktop\proyecto excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lfern\Desktop\clone repository\project-excel-versiones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9205F6A-F48C-4685-A3C6-66902FB710D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6CEE175-E8EF-4D2F-8308-D2F76A404C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F113BF61-DC04-49C9-8BD3-5B850611F5D3}"/>
+    <workbookView xWindow="6600" yWindow="2232" windowWidth="17280" windowHeight="8880" xr2:uid="{F113BF61-DC04-49C9-8BD3-5B850611F5D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -416,9 +416,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Subida con archivo modificado a rama 2
</commit_message>
<xml_diff>
--- a/project excel.xlsx
+++ b/project excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lfern\Desktop\clone repository\project-excel-versiones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6CEE175-E8EF-4D2F-8308-D2F76A404C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5CACC9-6301-45FB-B47F-C0AB86E781C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6600" yWindow="2232" windowWidth="17280" windowHeight="8880" xr2:uid="{F113BF61-DC04-49C9-8BD3-5B850611F5D3}"/>
+    <workbookView xWindow="540" yWindow="4728" windowWidth="17280" windowHeight="8880" xr2:uid="{F113BF61-DC04-49C9-8BD3-5B850611F5D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>My first project on excel</t>
+    <t xml:space="preserve">My first project on excel 2 </t>
   </si>
 </sst>
 </file>
@@ -412,9 +412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{657CCC46-E535-4C88-9957-5507C7534733}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>
   <sheetData>

</xml_diff>